<commit_message>
login form and remove chat link
</commit_message>
<xml_diff>
--- a/competitor_research/השוואת_טיולים_לפי_יעד.xlsx
+++ b/competitor_research/השוואת_טיולים_לפי_יעד.xlsx
@@ -1027,7 +1027,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1089,6 +1089,9 @@
       <c r="F6" t="str">
         <v>הערות</v>
       </c>
+      <c r="G6" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -1107,19 +1110,73 @@
         <v>—</v>
       </c>
       <c r="F7" t="str">
-        <v/>
+        <v>מאמרים והמלצות באתר</v>
+      </c>
+      <c r="G7" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>קשרי תעופה</v>
+      </c>
+      <c r="B8" t="str">
+        <v>שייט מאורגן לים הבלטי</v>
+      </c>
+      <c r="C8" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D8" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E8" t="str">
+        <v>—</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>קשרי תעופה</v>
+      </c>
+      <c r="B9" t="str">
+        <v>שייט מאוסטרלנד / שטוקהולם</v>
+      </c>
+      <c r="C9" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D9" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E9" t="str">
+        <v>—</v>
+      </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <v>קישור</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G7" r:id="rId1"/>
+    <hyperlink ref="G8" r:id="rId2"/>
+    <hyperlink ref="G9" r:id="rId3"/>
+  </hyperlinks>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1181,6 +1238,9 @@
       <c r="F6" t="str">
         <v>הערות</v>
       </c>
+      <c r="G6" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -1201,6 +1261,9 @@
       <c r="F7" t="str">
         <v/>
       </c>
+      <c r="G7" t="str">
+        <v/>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -1221,6 +1284,9 @@
       <c r="F8" t="str">
         <v/>
       </c>
+      <c r="G8" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -1241,6 +1307,9 @@
       <c r="F9" t="str">
         <v/>
       </c>
+      <c r="G9" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -1261,6 +1330,9 @@
       <c r="F10" t="str">
         <v/>
       </c>
+      <c r="G10" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -1281,6 +1353,9 @@
       <c r="F11" t="str">
         <v/>
       </c>
+      <c r="G11" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -1301,6 +1376,9 @@
       <c r="F12" t="str">
         <v/>
       </c>
+      <c r="G12" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -1321,6 +1399,9 @@
       <c r="F13" t="str">
         <v/>
       </c>
+      <c r="G13" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -1341,6 +1422,9 @@
       <c r="F14" t="str">
         <v/>
       </c>
+      <c r="G14" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -1361,6 +1445,9 @@
       <c r="F15" t="str">
         <v/>
       </c>
+      <c r="G15" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -1381,6 +1468,9 @@
       <c r="F16" t="str">
         <v/>
       </c>
+      <c r="G16" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -1401,6 +1491,9 @@
       <c r="F17" t="str">
         <v/>
       </c>
+      <c r="G17" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -1420,6 +1513,9 @@
       </c>
       <c r="F18" t="str">
         <v/>
+      </c>
+      <c r="G18" t="str">
+        <v>קישור</v>
       </c>
     </row>
     <row r="19">
@@ -1441,6 +1537,9 @@
       <c r="F19" t="str">
         <v>מובטח</v>
       </c>
+      <c r="G19" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -1461,6 +1560,9 @@
       <c r="F20" t="str">
         <v>מובטח</v>
       </c>
+      <c r="G20" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -1481,6 +1583,9 @@
       <c r="F21" t="str">
         <v>מובטח</v>
       </c>
+      <c r="G21" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -1501,6 +1606,9 @@
       <c r="F22" t="str">
         <v>מובטח</v>
       </c>
+      <c r="G22" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1521,6 +1629,9 @@
       <c r="F23" t="str">
         <v/>
       </c>
+      <c r="G23" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -1541,6 +1652,9 @@
       <c r="F24" t="str">
         <v/>
       </c>
+      <c r="G24" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1561,17 +1675,40 @@
       <c r="F25" t="str">
         <v/>
       </c>
+      <c r="G25" t="str">
+        <v>קישור</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1"/>
+    <hyperlink ref="G9" r:id="rId2"/>
+    <hyperlink ref="G10" r:id="rId3"/>
+    <hyperlink ref="G11" r:id="rId4"/>
+    <hyperlink ref="G12" r:id="rId5"/>
+    <hyperlink ref="G13" r:id="rId6"/>
+    <hyperlink ref="G14" r:id="rId7"/>
+    <hyperlink ref="G15" r:id="rId8"/>
+    <hyperlink ref="G16" r:id="rId9"/>
+    <hyperlink ref="G17" r:id="rId10"/>
+    <hyperlink ref="G18" r:id="rId11"/>
+    <hyperlink ref="G19" r:id="rId12"/>
+    <hyperlink ref="G20" r:id="rId13"/>
+    <hyperlink ref="G21" r:id="rId14"/>
+    <hyperlink ref="G22" r:id="rId15"/>
+    <hyperlink ref="G23" r:id="rId16"/>
+    <hyperlink ref="G24" r:id="rId17"/>
+    <hyperlink ref="G25" r:id="rId18"/>
+  </hyperlinks>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G25"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1633,13 +1770,16 @@
       <c r="F6" t="str">
         <v>הערות</v>
       </c>
+      <c r="G6" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
         <v>קרוזתור</v>
       </c>
       <c r="B7" t="str">
-        <v>שייט מאורגן לפיורדים</v>
+        <v>קרוז לפיורדים הנורבגיים (עם לונדון)</v>
       </c>
       <c r="C7" t="str">
         <v>באתר</v>
@@ -1653,37 +1793,95 @@
       <c r="F7" t="str">
         <v>מדריך עברית, סיורי חוף כלולים</v>
       </c>
+      <c r="G7" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
+        <v>קרוזתור</v>
+      </c>
+      <c r="B8" t="str">
+        <v>שייט מאורגן לפיורדים – תאריכים לפי חודש</v>
+      </c>
+      <c r="C8" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D8" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E8" t="str">
+        <v>פברואר–נובמבר 2026</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>קשרי תעופה</v>
+      </c>
+      <c r="B9" t="str">
+        <v>שייט מאורגן לפיורדים הנורבגיים</v>
+      </c>
+      <c r="C9" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D9" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E9" t="str">
+        <v>—</v>
+      </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
         <v>גולדן טורס</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B10" t="str">
         <v>קרוזים כשרים לפיורדים</v>
       </c>
-      <c r="C8" t="str">
-        <v>באתר</v>
-      </c>
-      <c r="D8" t="str">
-        <v>באתר</v>
-      </c>
-      <c r="E8" t="str">
+      <c r="C10" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D10" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E10" t="str">
         <v>—</v>
       </c>
-      <c r="F8" t="str">
-        <v/>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <v>קישור</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G7" r:id="rId1"/>
+    <hyperlink ref="G8" r:id="rId2"/>
+    <hyperlink ref="G9" r:id="rId3"/>
+    <hyperlink ref="G10" r:id="rId4"/>
+  </hyperlinks>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G10"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1759,25 +1957,31 @@
       <c r="F7" t="str">
         <v>הערות</v>
       </c>
+      <c r="G7" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <v>קרוזתור</v>
       </c>
       <c r="B8" t="str">
-        <v>קרוז לסינגפור, ויטנאם, הונג קונג, טאיוואן ויפן</v>
+        <v>ויטנאם וקמבודיה כולל שייט על המקונג</v>
       </c>
       <c r="C8" t="str">
-        <v>20</v>
+        <v>באתר</v>
       </c>
       <c r="D8" t="str">
         <v>באתר</v>
       </c>
       <c r="E8" t="str">
-        <v>פברואר 2027</v>
+        <v>—</v>
       </c>
       <c r="F8" t="str">
         <v/>
+      </c>
+      <c r="G8" t="str">
+        <v>קישור</v>
       </c>
     </row>
     <row r="9">
@@ -1785,19 +1989,22 @@
         <v>קרוזתור</v>
       </c>
       <c r="B9" t="str">
-        <v>שייט ליפן, טאיוואן, הפיליפינים והונג קונג</v>
+        <v>קרוז לסינגפור, ויטנאם, הונג קונג, טאיוואן ויפן</v>
       </c>
       <c r="C9" t="str">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9" t="str">
         <v>באתר</v>
       </c>
       <c r="E9" t="str">
-        <v>21/11/25</v>
+        <v>פברואר 2027</v>
       </c>
       <c r="F9" t="str">
         <v/>
+      </c>
+      <c r="G9" t="str">
+        <v>קישור</v>
       </c>
     </row>
     <row r="10">
@@ -1805,31 +2012,111 @@
         <v>קרוזתור</v>
       </c>
       <c r="B10" t="str">
+        <v>שייט ליפן, טאיוואן, הפיליפינים והונג קונג</v>
+      </c>
+      <c r="C10" t="str">
+        <v>18</v>
+      </c>
+      <c r="D10" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E10" t="str">
+        <v>21/11/25</v>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>קרוזתור</v>
+      </c>
+      <c r="B11" t="str">
+        <v>שייט למזרח הרחוק – אזור אסיה</v>
+      </c>
+      <c r="C11" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D11" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E11" t="str">
+        <v>—</v>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>קרוזתור</v>
+      </c>
+      <c r="B12" t="str">
         <v>שייט להונג קונג, הפיליפינים, טאיוואן ויפן</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C12" t="str">
         <v>21</v>
       </c>
-      <c r="D10" t="str">
-        <v>באתר</v>
-      </c>
-      <c r="E10" t="str">
+      <c r="D12" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E12" t="str">
         <v>פברואר 2026</v>
       </c>
-      <c r="F10" t="str">
-        <v/>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>קשרי תעופה</v>
+      </c>
+      <c r="B13" t="str">
+        <v>שייט למזרח הרחוק</v>
+      </c>
+      <c r="C13" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D13" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E13" t="str">
+        <v>—</v>
+      </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <v>קישור</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1"/>
+    <hyperlink ref="G9" r:id="rId2"/>
+    <hyperlink ref="G10" r:id="rId3"/>
+    <hyperlink ref="G11" r:id="rId4"/>
+    <hyperlink ref="G12" r:id="rId5"/>
+    <hyperlink ref="G13" r:id="rId6"/>
+  </hyperlinks>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G13"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1905,13 +2192,16 @@
       <c r="F7" t="str">
         <v>הערות</v>
       </c>
+      <c r="G7" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <v>קרוזתור</v>
       </c>
       <c r="B8" t="str">
-        <v>שייט מאורגן דנובה/מיין</v>
+        <v>שייט בנהר הדנובה עם משה דץ והזמרת שרי</v>
       </c>
       <c r="C8" t="str">
         <v>9</v>
@@ -1923,18 +2213,21 @@
         <v>—</v>
       </c>
       <c r="F8" t="str">
-        <v>סיורי חוף כלולים</v>
+        <v>מבודפשט לפסאו, סיורי חוף כלולים</v>
+      </c>
+      <c r="G8" t="str">
+        <v>קישור</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>גולדן טורס</v>
+        <v>קרוזתור</v>
       </c>
       <c r="B9" t="str">
-        <v>קרוזים כשרים לדנובה</v>
+        <v>שייט בנהר המיין ויובליו – הריין, בוואריה והדנובה</v>
       </c>
       <c r="C9" t="str">
-        <v>באתר</v>
+        <v>9</v>
       </c>
       <c r="D9" t="str">
         <v>באתר</v>
@@ -1943,19 +2236,74 @@
         <v>—</v>
       </c>
       <c r="F9" t="str">
-        <v/>
+        <v>עם להקת הגבעטרון ומשה דץ</v>
+      </c>
+      <c r="G9" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>קרוזתור</v>
+      </c>
+      <c r="B10" t="str">
+        <v>שייט מאורגן על הדנובה – תאריכים לפי חודש</v>
+      </c>
+      <c r="C10" t="str">
+        <v>9</v>
+      </c>
+      <c r="D10" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E10" t="str">
+        <v>פברואר–ינואר 2027</v>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>גולדן טורס</v>
+      </c>
+      <c r="B11" t="str">
+        <v>קרוזים כשרים לדנובה</v>
+      </c>
+      <c r="C11" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D11" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E11" t="str">
+        <v>—</v>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <v>קישור</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1"/>
+    <hyperlink ref="G9" r:id="rId2"/>
+    <hyperlink ref="G10" r:id="rId3"/>
+    <hyperlink ref="G11" r:id="rId4"/>
+  </hyperlinks>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G11"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2045,37 +2393,70 @@
       <c r="F8" t="str">
         <v>הערות</v>
       </c>
+      <c r="G8" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>—</v>
+        <v>קרוזתור</v>
       </c>
       <c r="B9" t="str">
-        <v>לא נמצאו טיולי דואורו במתחרים בסריקה</v>
+        <v>שייט בנהר הדואורו בפורטוגל</v>
       </c>
       <c r="C9" t="str">
-        <v>—</v>
+        <v>באתר</v>
       </c>
       <c r="D9" t="str">
-        <v>—</v>
+        <v>באתר</v>
       </c>
       <c r="E9" t="str">
         <v>—</v>
       </c>
       <c r="F9" t="str">
-        <v/>
+        <v>סיורי חוף כלולים, מדריך עברית</v>
+      </c>
+      <c r="G9" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>קשרי תעופה</v>
+      </c>
+      <c r="B10" t="str">
+        <v>שייט נהרות בפורטוגל (דואורו)</v>
+      </c>
+      <c r="C10" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D10" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E10" t="str">
+        <v>—</v>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <v>קישור</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G9" r:id="rId1"/>
+    <hyperlink ref="G10" r:id="rId2"/>
+  </hyperlinks>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G10"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2151,16 +2532,19 @@
       <c r="F7" t="str">
         <v>הערות</v>
       </c>
+      <c r="G7" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>מנו ספנות</v>
+        <v>קרוזתור</v>
       </c>
       <c r="B8" t="str">
-        <v>קרוזים לים התיכון (הפלגה מחיפה)</v>
+        <v>קרוז מאורגן למערב הים התיכון ואגמי צפון איטליה</v>
       </c>
       <c r="C8" t="str">
-        <v>באתר</v>
+        <v>11</v>
       </c>
       <c r="D8" t="str">
         <v>באתר</v>
@@ -2169,7 +2553,10 @@
         <v>—</v>
       </c>
       <c r="F8" t="str">
-        <v>סיורי חוף, כשר</v>
+        <v>גנואה, סיציליה, מלטה, ברצלונה, אקס אן פרובנס, מילאנו</v>
+      </c>
+      <c r="G8" t="str">
+        <v>קישור</v>
       </c>
     </row>
     <row r="9">
@@ -2177,7 +2564,7 @@
         <v>קרוזתור</v>
       </c>
       <c r="B9" t="str">
-        <v>שייט מאורגן ים תיכון</v>
+        <v>קרוז בים התיכון – אזור הים התיכון</v>
       </c>
       <c r="C9" t="str">
         <v>באתר</v>
@@ -2191,17 +2578,144 @@
       <c r="F9" t="str">
         <v>סיורי חוף כלולים</v>
       </c>
+      <c r="G9" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>קשרי תעופה</v>
+      </c>
+      <c r="B10" t="str">
+        <v>שייט מאורגן בצפון מערב אירופה</v>
+      </c>
+      <c r="C10" t="str">
+        <v>10</v>
+      </c>
+      <c r="D10" t="str">
+        <v>$4,595</v>
+      </c>
+      <c r="E10" t="str">
+        <v>28/05/26</v>
+      </c>
+      <c r="F10" t="str">
+        <v>פנסיון מלא, Celebrity Apex</v>
+      </c>
+      <c r="G10" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>קשרי תעופה</v>
+      </c>
+      <c r="B11" t="str">
+        <v>שייט רביירות ים תיכון</v>
+      </c>
+      <c r="C11" t="str">
+        <v>9</v>
+      </c>
+      <c r="D11" t="str">
+        <v>$3,695</v>
+      </c>
+      <c r="E11" t="str">
+        <v>31/07/26</v>
+      </c>
+      <c r="F11" t="str">
+        <v>MSC Seaview</v>
+      </c>
+      <c r="G11" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>קשרי תעופה</v>
+      </c>
+      <c r="B12" t="str">
+        <v>שייט רביירות מערב אירופה</v>
+      </c>
+      <c r="C12" t="str">
+        <v>7</v>
+      </c>
+      <c r="D12" t="str">
+        <v>$3,499</v>
+      </c>
+      <c r="E12" t="str">
+        <v>16/08/26</v>
+      </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>קשרי תעופה</v>
+      </c>
+      <c r="B13" t="str">
+        <v>שייט ריביירות מערב אירופה סוכות</v>
+      </c>
+      <c r="C13" t="str">
+        <v>7</v>
+      </c>
+      <c r="D13" t="str">
+        <v>$3,595</v>
+      </c>
+      <c r="E13" t="str">
+        <v>27/09/26</v>
+      </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>מנו ספנות</v>
+      </c>
+      <c r="B14" t="str">
+        <v>קרוזים לים התיכון (הפלגה מחיפה)</v>
+      </c>
+      <c r="C14" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D14" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E14" t="str">
+        <v>—</v>
+      </c>
+      <c r="F14" t="str">
+        <v>סיורי חוף, כשר</v>
+      </c>
+      <c r="G14" t="str">
+        <v>קישור</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1"/>
+    <hyperlink ref="G9" r:id="rId2"/>
+    <hyperlink ref="G10" r:id="rId3"/>
+    <hyperlink ref="G11" r:id="rId4"/>
+    <hyperlink ref="G12" r:id="rId5"/>
+    <hyperlink ref="G13" r:id="rId6"/>
+    <hyperlink ref="G14" r:id="rId7"/>
+  </hyperlinks>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G14"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2263,13 +2777,16 @@
       <c r="F6" t="str">
         <v>הערות</v>
       </c>
+      <c r="G6" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
         <v>קרוזתור</v>
       </c>
       <c r="B7" t="str">
-        <v>קרוזים לקנדה מערב ואלסקה / איים בריטיים</v>
+        <v>קרוז לאלסקה וטיול להרי הרוקי הקנדיים</v>
       </c>
       <c r="C7" t="str">
         <v>באתר</v>
@@ -2283,17 +2800,71 @@
       <c r="F7" t="str">
         <v/>
       </c>
+      <c r="G7" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>קרוזתור</v>
+      </c>
+      <c r="B8" t="str">
+        <v>קרוז לאלסקה והרי הרוקי</v>
+      </c>
+      <c r="C8" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D8" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E8" t="str">
+        <v>—</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>קשרי תעופה</v>
+      </c>
+      <c r="B9" t="str">
+        <v>שייט מאורגן לאלסקה</v>
+      </c>
+      <c r="C9" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D9" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E9" t="str">
+        <v>—</v>
+      </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <v>קישור</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G7" r:id="rId1"/>
+    <hyperlink ref="G8" r:id="rId2"/>
+    <hyperlink ref="G9" r:id="rId3"/>
+  </hyperlinks>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2411,16 +2982,19 @@
       <c r="F10" t="str">
         <v>הערות</v>
       </c>
+      <c r="G10" t="str">
+        <v>קישור</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>גולדן טורס</v>
+        <v>קרוזתור</v>
       </c>
       <c r="B11" t="str">
-        <v>קרוזים כשרים לריין, דנובה</v>
+        <v>שייט בנהר המיין ויובליו – הריין, בוואריה והדנובה</v>
       </c>
       <c r="C11" t="str">
-        <v>באתר</v>
+        <v>9</v>
       </c>
       <c r="D11" t="str">
         <v>באתר</v>
@@ -2429,7 +3003,10 @@
         <v>—</v>
       </c>
       <c r="F11" t="str">
-        <v/>
+        <v>עם להקת הגבעטרון ומשה דץ</v>
+      </c>
+      <c r="G11" t="str">
+        <v>קישור</v>
       </c>
     </row>
     <row r="12">
@@ -2437,10 +3014,10 @@
         <v>קרוזתור</v>
       </c>
       <c r="B12" t="str">
-        <v>שייט נהרות מאורגן (דנובה, מיין וכו')</v>
+        <v>שייט בנהר הסיין בצרפת</v>
       </c>
       <c r="C12" t="str">
-        <v>9</v>
+        <v>באתר</v>
       </c>
       <c r="D12" t="str">
         <v>באתר</v>
@@ -2451,10 +3028,161 @@
       <c r="F12" t="str">
         <v/>
       </c>
+      <c r="G12" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>קרוזתור</v>
+      </c>
+      <c r="B13" t="str">
+        <v>שייט בנהרות הרון והסון בצרפת</v>
+      </c>
+      <c r="C13" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D13" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E13" t="str">
+        <v>—</v>
+      </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>קרוזתור</v>
+      </c>
+      <c r="B14" t="str">
+        <v>שייט על הריין ועל המוזל</v>
+      </c>
+      <c r="C14" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D14" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E14" t="str">
+        <v>—</v>
+      </c>
+      <c r="F14" t="str">
+        <v/>
+      </c>
+      <c r="G14" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>קרוזתור</v>
+      </c>
+      <c r="B15" t="str">
+        <v>שייט נהרות בצרפת (סיין, רון, דורדון)</v>
+      </c>
+      <c r="C15" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D15" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E15" t="str">
+        <v>—</v>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>קרוזתור</v>
+      </c>
+      <c r="B16" t="str">
+        <v>שייט נהרות בהולנד ובלגיה</v>
+      </c>
+      <c r="C16" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D16" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E16" t="str">
+        <v>—</v>
+      </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>גולדן טורס</v>
+      </c>
+      <c r="B17" t="str">
+        <v>קרוזים כשרים לריין, דנובה</v>
+      </c>
+      <c r="C17" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="D17" t="str">
+        <v>באתר</v>
+      </c>
+      <c r="E17" t="str">
+        <v>—</v>
+      </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
+      <c r="G17" t="str">
+        <v>קישור</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>קשרי תעופה</v>
+      </c>
+      <c r="B18" t="str">
+        <v>שייט מאורגן ריביירות (ים תיכון/מערב אירופה)</v>
+      </c>
+      <c r="C18" t="str">
+        <v>7–10</v>
+      </c>
+      <c r="D18" t="str">
+        <v>$3,499–$4,595</v>
+      </c>
+      <c r="E18" t="str">
+        <v>2026</v>
+      </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <v>קישור</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G11" r:id="rId1"/>
+    <hyperlink ref="G12" r:id="rId2"/>
+    <hyperlink ref="G13" r:id="rId3"/>
+    <hyperlink ref="G14" r:id="rId4"/>
+    <hyperlink ref="G15" r:id="rId5"/>
+    <hyperlink ref="G16" r:id="rId6"/>
+    <hyperlink ref="G17" r:id="rId7"/>
+    <hyperlink ref="G18" r:id="rId8"/>
+  </hyperlinks>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>